<commit_message>
part 3- trying to make taxon checking more efficient setting up for matching of distinct names. Adding folders to house taxonomy reference data
</commit_message>
<xml_diff>
--- a/data/digitized_data/occurrence_data/raw_data/HJ-5-occ-entry.xlsx
+++ b/data/digitized_data/occurrence_data/raw_data/HJ-5-occ-entry.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emma/Desktop/LDP Internship/Harvey_Janszen_Legacy_Project/data/digitized_data/occurrence_data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF26414-F8BA-2A4B-BB90-48052F8B856E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{234C6F66-ABC5-4746-8E14-62B575046987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15400" xr2:uid="{6CD260D0-3248-EC4C-A246-EE521030FA00}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15340" xr2:uid="{6CD260D0-3248-EC4C-A246-EE521030FA00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3169,10 +3169,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E2B542-A597-DF4D-A726-D9C00BB4087B}">
   <dimension ref="A1:AH64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="171" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="171" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3464,7 +3464,9 @@
       <c r="AH5"/>
     </row>
     <row r="6" spans="1:34" ht="51" x14ac:dyDescent="0.2">
-      <c r="B6"/>
+      <c r="B6">
+        <v>11</v>
+      </c>
       <c r="C6"/>
       <c r="D6" t="s">
         <v>48</v>
@@ -3499,7 +3501,9 @@
       <c r="AH6"/>
     </row>
     <row r="7" spans="1:34" ht="68" x14ac:dyDescent="0.2">
-      <c r="B7"/>
+      <c r="B7">
+        <v>11</v>
+      </c>
       <c r="C7"/>
       <c r="D7"/>
       <c r="E7"/>

</xml_diff>

<commit_message>
revising occurrence entry templates to include qualifier id
</commit_message>
<xml_diff>
--- a/data/digitized_data/occurrence_data/raw_data/HJ-5-occ-entry.xlsx
+++ b/data/digitized_data/occurrence_data/raw_data/HJ-5-occ-entry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emma/Desktop/LDP Internship/Harvey_Janszen_Legacy_Project/data/digitized_data/occurrence_data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{234C6F66-ABC5-4746-8E14-62B575046987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA54601-72D1-324A-9EC4-78D066AC39D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15340" xr2:uid="{6CD260D0-3248-EC4C-A246-EE521030FA00}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="pageNum" comment="page number of field journal (each side of a page as a new number so the front and back of the first page would be 1, and 2 respectively">Sheet1!$B$1</definedName>
+    <definedName name="pageNum" comment="page number of field journal (each side of a page as a new number so the front and back of the first page would be 1, and 2 respectively">Sheet1!$A$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,77 +41,95 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>Emma Menchions</author>
     <author>Kyle Braak</author>
-    <author>Emma Menchions</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{F97510D6-8FCC-3F44-9194-E70FA9344A77}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{A8DDB6DB-164F-B542-BF28-66A88C3A6BAE}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">archiveID (REQUIRED)
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Definition:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">  The number associated with the field journal representing a unique item in the archive, with a dash between "HJ" and the number
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Example: HJ-27</t>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">pageNum (REQURIED)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Definition: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Page number of field journal. Each side of a page is a new number 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Example</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>: front and back side of first page are numbers 1 and 2 respectively</t>
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="1" shapeId="0" xr:uid="{A8DDB6DB-164F-B542-BF28-66A88C3A6BAE}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{C4C6551D-B61A-0F47-BF4B-625CAEB4EF97}">
       <text>
         <r>
           <rPr>
@@ -121,21 +139,23 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">pageNum (REQURIED)
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
+          <t xml:space="preserve">numPage (REQUIRED)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
@@ -161,41 +181,41 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Page number of field journal. Each side of a page is a new number 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Example</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>: front and back side of first page are numbers 1 and 2 respectively</t>
+          <t xml:space="preserve">the number of the observation on a given page (in order).
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Example: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The first species name/ observation on the page excluding collected observations on the page = 1. Alternatively it can refer to observations of associated taxa in collected specimen notes. </t>
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="1" shapeId="0" xr:uid="{C4C6551D-B61A-0F47-BF4B-625CAEB4EF97}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{552BA6F0-B4A1-3441-A7FC-6A6D93AA887E}">
       <text>
         <r>
           <rPr>
@@ -205,7 +225,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">numPage (REQUIRED)
+          <t xml:space="preserve">vName (REQUIRED)
 </t>
         </r>
         <r>
@@ -247,7 +267,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">the number of the observation on a given page (in order).
+          <t xml:space="preserve">the verbatim name written in the field journal. Might be an abbreviation or the full name 
 </t>
         </r>
         <r>
@@ -274,14 +294,36 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The first species name/ observation on the page excluding collected observations on the page = 1. Alternatively it can refer to observations of associated taxa in collected specimen notes. </t>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Stel med, Elodea densa
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="1" shapeId="0" xr:uid="{552BA6F0-B4A1-3441-A7FC-6A6D93AA887E}">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{B42992FB-531D-9743-ADA0-2BD04AFE5FCA}">
       <text>
         <r>
           <rPr>
@@ -291,49 +333,75 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">vName (REQUIRED)
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Definition: </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">the verbatim name written in the field journal. Might be an abbreviation or the full name 
+          <t>vSciName (REQUIRED)</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Defintiion: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">your estimation of what the verbatim scientific taxon name is based on the vName. </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Can just be a genus or family name if not confident in deciphering specific epiphet or it is not provided. Might be a repeat of the vName field if it was not an abbreviation.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
 </t>
         </r>
         <r>
@@ -360,36 +428,14 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Stel med, Elodea densa
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Stellaria media, Elodea densa</t>
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="1" shapeId="0" xr:uid="{B42992FB-531D-9743-ADA0-2BD04AFE5FCA}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{C737CA67-21CB-4540-AEE9-D83B28E161DB}">
       <text>
         <r>
           <rPr>
@@ -399,75 +445,89 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>vSciName (REQUIRED)</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Defintiion: </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">your estimation of what the verbatim scientific taxon name is based on the vName. </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Can just be a genus or family name if not confident in deciphering specific epiphet or it is not provided. Might be a repeat of the vName field if it was not an abbreviation.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
+          <t xml:space="preserve">Conf (REQUIRED)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Definition: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">your level of confidence in assigning a full taxon name to the abbreviation/ fully written name that is hard to decipher
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">"l" = low confidence and should be checked over
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">"m" = medium confidence and should be checked over if there is time but not prioritized
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">"h" = high confidence and likely does not need to be checked
 </t>
         </r>
         <r>
@@ -497,11 +557,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Stellaria media, Elodea densa</t>
+          <t>m</t>
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="1" shapeId="0" xr:uid="{C737CA67-21CB-4540-AEE9-D83B28E161DB}">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{274940BF-7D64-7141-8417-AC7302876D53}">
       <text>
         <r>
           <rPr>
@@ -511,7 +571,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Conf (REQUIRED)
+          <t xml:space="preserve">sciName (REQUIRED)
 </t>
         </r>
         <r>
@@ -553,81 +613,62 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">your level of confidence in assigning a full taxon name to the abbreviation/ fully written name that is hard to decipher
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">"l" = low confidence and should be checked over
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">"m" = medium confidence and should be checked over if there is time but not prioritized
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">"h" = high confidence and likely does not need to be checked
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Example: </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>m</t>
+          <t xml:space="preserve">up to date taxon name based on iNaturalist definitions. If the verbatim scientific name has been updated to a new name, record this here. Alternatively if there is no change, copy the verbatim name to this column. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Example: "</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Osmorhiza berteroi" (updated from vSciName of Osmorhiza chilensis</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="1" shapeId="0" xr:uid="{274940BF-7D64-7141-8417-AC7302876D53}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{DEAEAD63-48ED-2A4E-9FA0-F8A60DF75BFA}">
       <text>
         <r>
           <rPr>
@@ -637,7 +678,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">sciName (REQUIRED)
+          <t xml:space="preserve">date (REQUIRED)
 </t>
         </r>
         <r>
@@ -679,62 +720,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">up to date taxon name based on iNaturalist definitions. If the verbatim scientific name has been updated to a new name, record this here. Alternatively if there is no change, copy the verbatim name to this column. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Example: "</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Osmorhiza berteroi" (updated from vSciName of Osmorhiza chilensis</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
+          <t>occurrence observation date. Entered in YYYYMMDD format. If none can be associated with an occurrence, do not enter the occurrence and skip to the next observation with a date</t>
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="1" shapeId="0" xr:uid="{DEAEAD63-48ED-2A4E-9FA0-F8A60DF75BFA}">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{DC1234B4-128B-9D44-9647-ACD44B00D397}">
       <text>
         <r>
           <rPr>
@@ -744,7 +734,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">date (REQUIRED)
+          <t xml:space="preserve">locality (REQUIRED)
 </t>
         </r>
         <r>
@@ -786,11 +776,81 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>occurrence observation date. Entered in YYYYMMDD format. If none can be associated with an occurrence, do not enter the occurrence and skip to the next observation with a date</t>
+          <t xml:space="preserve">string of letters indicating a specific location. Does not contain country, province, county/ municipality information but includes the name of an island, town, local landmark, road etc.Try to spell out abbreciations for Rd, Mt.  
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Example: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Mount Sutil, Galiano Island
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">NOT 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mount Sutil, Galiano Island, Southern Gulf Islands, British Columbia, Canada (this is okay to do but not necessary)</t>
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="1" shapeId="0" xr:uid="{DC1234B4-128B-9D44-9647-ACD44B00D397}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{144860E7-37A9-7442-9661-FC5E9C626D31}">
       <text>
         <r>
           <rPr>
@@ -800,7 +860,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">locality (REQUIRED)
+          <t xml:space="preserve">country (REQUIRED) 
 </t>
         </r>
         <r>
@@ -842,7 +902,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">string of letters indicating a specific location. Does not contain country, province, county/ municipality information but includes the name of an island, town, local landmark, road etc.Try to spell out abbreciations for Rd, Mt.  
+          <t xml:space="preserve">country of collection
 </t>
         </r>
         <r>
@@ -872,51 +932,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Mount Sutil, Galiano Island
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">NOT 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Mount Sutil, Galiano Island, Southern Gulf Islands, British Columbia, Canada (this is okay to do but not necessary)</t>
+          <t>either United States or Canada</t>
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="1" shapeId="0" xr:uid="{144860E7-37A9-7442-9661-FC5E9C626D31}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{69A0DE11-3D9B-DD45-BD54-68EAC4E3B77F}">
       <text>
         <r>
           <rPr>
@@ -926,7 +946,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">country (REQUIRED) 
+          <t xml:space="preserve">stateProvince (REQUIRED)
 </t>
         </r>
         <r>
@@ -968,7 +988,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">country of collection
+          <t xml:space="preserve">province or state occurrence was observed in 
 </t>
         </r>
         <r>
@@ -998,11 +1018,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>either United States or Canada</t>
+          <t>British Columbia or Washington</t>
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="1" shapeId="0" xr:uid="{69A0DE11-3D9B-DD45-BD54-68EAC4E3B77F}">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{FA07C549-45F1-6843-BD8A-5C29B980EF43}">
       <text>
         <r>
           <rPr>
@@ -1012,7 +1032,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">stateProvince (REQUIRED)
+          <t xml:space="preserve">island (REQUIRED)
 </t>
         </r>
         <r>
@@ -1054,41 +1074,41 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">province or state occurrence was observed in 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Example: </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>British Columbia or Washington</t>
+          <t xml:space="preserve">island on which the occurrence was observed
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Examples: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Vancouver Island, Saltspring, Galiano, Texada</t>
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="1" shapeId="0" xr:uid="{FA07C549-45F1-6843-BD8A-5C29B980EF43}">
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{56E53AC6-F7E8-414E-9269-60273345448B}">
       <text>
         <r>
           <rPr>
@@ -1098,7 +1118,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">island (REQUIRED)
+          <t xml:space="preserve">county (REQUIRED)
 </t>
         </r>
         <r>
@@ -1140,7 +1160,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">island on which the occurrence was observed
+          <t xml:space="preserve">county/ municipality that occurrence was observed in.
 </t>
         </r>
         <r>
@@ -1170,11 +1190,12 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Vancouver Island, Saltspring, Galiano, Texada</t>
+          <t xml:space="preserve">Southern Gulf Islands, Northern Gulf Islands, Victoria, Saanich, Metchosin, Sidney
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="1" shapeId="0" xr:uid="{56E53AC6-F7E8-414E-9269-60273345448B}">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{0262923D-9B4C-7E48-B57E-DC6FA182E66C}">
       <text>
         <r>
           <rPr>
@@ -1184,84 +1205,83 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">county (REQUIRED)
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Definition: </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">county/ municipality that occurrence was observed in.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Examples: </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Southern Gulf Islands, Northern Gulf Islands, Victoria, Saanich, Metchosin, Sidney
-</t>
+          <t xml:space="preserve">occStaus (REQUIRED)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Definition: occurrence status. </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">indicates whether the species was observed to be present or absent
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Example: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">If special note made about specific taxon not being at a given location = "absent". Otherwise = "present" </t>
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="1" shapeId="0" xr:uid="{0262923D-9B4C-7E48-B57E-DC6FA182E66C}">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{D02977E1-488B-9F48-A6C9-AB421B4FC449}">
       <text>
         <r>
           <rPr>
@@ -1271,83 +1291,75 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">occStaus (REQUIRED)
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Definition: occurrence status. </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">indicates whether the species was observed to be present or absent
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Example: </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">If special note made about specific taxon not being at a given location = "absent". Otherwise = "present" </t>
+          <t xml:space="preserve">locationRemarks
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Definition: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Use this column to denote information about plot location or polygon number, or miscellaneous notes that discuss the relative position or the state of the habitat/ site
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Example: poly 20
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="1" shapeId="0" xr:uid="{D02977E1-488B-9F48-A6C9-AB421B4FC449}">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{C09603FC-3352-834C-B4F5-F61FDEF58211}">
       <text>
         <r>
           <rPr>
@@ -1357,75 +1369,64 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">locationRemarks
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Definition: </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Use this column to denote information about plot location or polygon number, or miscellaneous notes that discuss the relative position or the state of the habitat/ site
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Example: poly 20
-</t>
+          <t xml:space="preserve">habitat 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Defintion: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>if habitat information provided, place here. This includes whether it is in an aquatic vs terrestrial habitat (aquatic, in lake shoreline), the biogeoclimatic zone, shading conditions (e.g. in shade, shaded, in sun) , relative position at locality (e.g. base vs seep vs ledge), position on habitat objects (e.g. on log)</t>
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="1" shapeId="0" xr:uid="{C09603FC-3352-834C-B4F5-F61FDEF58211}">
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{600D10A9-A6C8-C642-81F6-27CD7835EAC6}">
       <text>
         <r>
           <rPr>
@@ -1435,64 +1436,94 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">habitat 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Defintion: </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>if habitat information provided, place here. This includes whether it is in an aquatic vs terrestrial habitat (aquatic, in lake shoreline), the biogeoclimatic zone, shading conditions (e.g. in shade, shaded, in sun) , relative position at locality (e.g. base vs seep vs ledge), position on habitat objects (e.g. on log)</t>
+          <t xml:space="preserve">vTaxonRank (REQUIRED)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Definition: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">verbatim taxon rank. The lowest level of taxonomy provided. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Example: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">if specific epiphet in scientific name = "species", alternatively if lowest level is generic name = "genus"
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="1" shapeId="0" xr:uid="{600D10A9-A6C8-C642-81F6-27CD7835EAC6}">
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{31FD17C0-D5AE-6F41-8345-1A4EFE68544A}">
       <text>
         <r>
           <rPr>
@@ -1502,23 +1533,30 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">vTaxonRank (REQUIRED)
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
+          <t>vElev</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
@@ -1544,145 +1582,137 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">verbatim taxon rank. The lowest level of taxonomy provided. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Example: </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">if specific epiphet in scientific name = "species", alternatively if lowest level is generic name = "genus"
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
+          <t xml:space="preserve">verbatim elevation. The elevation in meters if provided
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Example</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">: 10 </t>
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="1" shapeId="0" xr:uid="{31FD17C0-D5AE-6F41-8345-1A4EFE68544A}">
+    <comment ref="S1" authorId="1" shapeId="0" xr:uid="{5B13E7B4-E6E7-D045-B018-8FAC95E81BC0}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>vElev</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Definition: </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">verbatim elevation. The elevation in meters if provided
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Example</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">: 10 </t>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">vLat 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Definition:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> verbatim latitude. The geographic latitude in decimal degrees or degrees minutes seconds. Positive values are north of the Equator, negative values are south of it. Legal values lie between -90 and 90, inclusive.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Examples: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> "-41.0983423". If degrees minutes seconds: 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>49 39 12</t>
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{5B13E7B4-E6E7-D045-B018-8FAC95E81BC0}">
+    <comment ref="T1" authorId="1" shapeId="0" xr:uid="{B05819FB-05BF-4342-8D04-1FDAFB40A3C0}">
       <text>
         <r>
           <rPr>
@@ -1692,7 +1722,7 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">vLat 
+          <t xml:space="preserve">RECOMMENDED
 </t>
         </r>
         <r>
@@ -1714,18 +1744,16 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
+          <t>Definition:</t>
+        </r>
+        <r>
+          <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t>Definition:</t>
+          <t xml:space="preserve"> </t>
         </r>
         <r>
           <rPr>
@@ -1733,9 +1761,9 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> verbatim latitude. The geographic latitude in decimal degrees or degrees minutes seconds. Positive values are north of the Equator, negative values are south of it. Legal values lie between -90 and 90, inclusive.
-</t>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">verbatim longitude. The geographic longitude in decimal degrees or degrees minutes seconds. </t>
         </r>
         <r>
           <rPr>
@@ -1744,17 +1772,27 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
+          <t xml:space="preserve">Positive values are east of the Greenwich Meridian, negative values are west of it. Legal values lie between -180 and 180, inclusive.
+</t>
+        </r>
+        <r>
+          <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
           <t xml:space="preserve">Examples: </t>
         </r>
         <r>
@@ -1764,115 +1802,85 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> "-41.0983423". If degrees minutes seconds: 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>49 39 12</t>
+          <t xml:space="preserve"> "-121.1761111". If in degrees minutes secons: 124 56 37</t>
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{B05819FB-05BF-4342-8D04-1FDAFB40A3C0}">
+    <comment ref="U1" authorId="0" shapeId="0" xr:uid="{00D86AB6-65FF-F44F-B9EE-5D02C7CDA473}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">RECOMMENDED
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Definition:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">verbatim longitude. The geographic longitude in decimal degrees or degrees minutes seconds. </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Positive values are east of the Greenwich Meridian, negative values are west of it. Legal values lie between -180 and 180, inclusive.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Examples: </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> "-121.1761111". If in degrees minutes secons: 124 56 37</t>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">vUTM
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Definition: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">if verbatim coordinates in UTM, denote in this column. Separate into 3 strings. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Example: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>10U 45689 55678</t>
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="1" shapeId="0" xr:uid="{00D86AB6-65FF-F44F-B9EE-5D02C7CDA473}">
+    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{2410207F-8B4D-4246-9450-D9FC90711A12}">
       <text>
         <r>
           <rPr>
@@ -1882,11 +1890,12 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">vUTM
-</t>
-        </r>
-        <r>
-          <rPr>
+          <t xml:space="preserve">vCoordUncertainty
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
@@ -1912,7 +1921,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">if verbatim coordinates in UTM, denote in this column. Separate into 3 strings. 
+          <t xml:space="preserve">denote the verbatim coordinate uncertainty in meters if provided with associated verbatim UTM or degree coordinates 
 </t>
         </r>
         <r>
@@ -1942,11 +1951,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>10U 45689 55678</t>
+          <t xml:space="preserve">30 </t>
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="1" shapeId="0" xr:uid="{2410207F-8B4D-4246-9450-D9FC90711A12}">
+    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{CD0706FF-5811-BF49-993E-D0941F3AA07B}">
       <text>
         <r>
           <rPr>
@@ -1956,7 +1965,18 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">vCoordUncertainty
+          <t xml:space="preserve">assTaxa
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
 </t>
         </r>
         <r>
@@ -1987,7 +2007,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">denote the verbatim coordinate uncertainty in meters if provided with associated verbatim UTM or degree coordinates 
+          <t xml:space="preserve">associated taxa. Use this field to denote scientific names of associated taxa. HOWEVER, only do this if that associated taxa has a collection number/ is a collected specimen. Otherwise leave blank. 
 </t>
         </r>
         <r>
@@ -2017,37 +2037,24 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">30 </t>
+          <t>Isoetes echinospora</t>
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="1" shapeId="0" xr:uid="{CD0706FF-5811-BF49-993E-D0941F3AA07B}">
+    <comment ref="X1" authorId="0" shapeId="0" xr:uid="{83478F65-73DB-E043-B4E7-852EE638A389}">
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">assTaxa
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">assOcc
+</t>
+        </r>
+        <r>
+          <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
@@ -2073,7 +2080,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">associated taxa. Use this field to denote scientific names of associated taxa. HOWEVER, only do this if that associated taxa has a collection number/ is a collected specimen. Otherwise leave blank. 
+          <t xml:space="preserve">the occurrence numbers of taxa growing with this occurrence. HOWEVER, when entering data, only input data in this column if occurrence was growing with a specimen that was collected. Record the collection number here with HJC to indicate collected specimen
 </t>
         </r>
         <r>
@@ -2103,143 +2110,144 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Isoetes echinospora</t>
+          <t>"HJC-2863"</t>
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="1" shapeId="0" xr:uid="{83478F65-73DB-E043-B4E7-852EE638A389}">
+    <comment ref="Y1" authorId="1" shapeId="0" xr:uid="{2B56D7A6-70C4-964C-B53F-5099151A0A9C}">
       <text>
         <r>
           <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">assOcc
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Definition: </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">the occurrence numbers of taxa growing with this occurrence. HOWEVER, when entering data, only input data in this column if occurrence was growing with a specimen that was collected. Record the collection number here with HJC to indicate collected specimen
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Example: </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>"HJC-2863"</t>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">RECOMMENDED
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Definition:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> The number of individuals represented present at the time of the Occurrence.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Examples: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> "1", "25".</t>
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="0" shapeId="0" xr:uid="{2B56D7A6-70C4-964C-B53F-5099151A0A9C}">
+    <comment ref="AB1" authorId="0" shapeId="0" xr:uid="{D0775F8C-E8A1-D240-B257-347544436168}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">RECOMMENDED
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Definition:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> The number of individuals represented present at the time of the Occurrence.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">occRemarks
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Definition: </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Remarks about the occurrence that do not fit into other columns. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">Examples: </t>
@@ -2248,14 +2256,14 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> "1", "25".</t>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>"abundant", "prevalent" , "no unusual travel off" "dominant" "very few" "add", "two large beds", "approx 30% cover"</t>
         </r>
       </text>
     </comment>
-    <comment ref="AB1" authorId="1" shapeId="0" xr:uid="{D0775F8C-E8A1-D240-B257-347544436168}">
+    <comment ref="AD1" authorId="0" shapeId="0" xr:uid="{6547EF21-25AE-6F4F-AF2D-4DBC5EF0E9B5}">
       <text>
         <r>
           <rPr>
@@ -2265,11 +2273,12 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">occRemarks
-</t>
-        </r>
-        <r>
-          <rPr>
+          <t xml:space="preserve">recordedBy
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
@@ -2295,7 +2304,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Remarks about the occurrence that do not fit into other columns. 
+          <t xml:space="preserve">who the occurrence data was recorded by. If more than one individual, separate names with "|"
 </t>
         </r>
         <r>
@@ -2325,11 +2334,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>"abundant", "prevalent" , "no unusual travel off" "dominant" "very few" "add", "two large beds", "approx 30% cover"</t>
+          <t>"Harvey Janszen", "Harvey Janszen" | "Pam Janszen"</t>
         </r>
       </text>
     </comment>
-    <comment ref="AD1" authorId="1" shapeId="0" xr:uid="{6547EF21-25AE-6F4F-AF2D-4DBC5EF0E9B5}">
+    <comment ref="AE1" authorId="0" shapeId="0" xr:uid="{7FD26A50-5CA6-FE43-83AC-339CADE77507}">
       <text>
         <r>
           <rPr>
@@ -2339,7 +2348,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">recordedBy
+          <t xml:space="preserve">idBy
 </t>
         </r>
         <r>
@@ -2370,87 +2379,12 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">who the occurrence data was recorded by. If more than one individual, separate names with "|"
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Examples: </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>"Harvey Janszen", "Harvey Janszen" | "Pam Janszen"</t>
+          <t xml:space="preserve">identification by. Who identified the occurrence as a particular taxon? Follow the same formatting for recordedBy field if more than one individual. 
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="AE1" authorId="1" shapeId="0" xr:uid="{7FD26A50-5CA6-FE43-83AC-339CADE77507}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">idBy
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Definition: </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">identification by. Who identified the occurrence as a particular taxon? Follow the same formatting for recordedBy field if more than one individual. 
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AF1" authorId="1" shapeId="0" xr:uid="{755321BC-C668-F042-8E31-CF64ED8C27AF}">
+    <comment ref="AF1" authorId="0" shapeId="0" xr:uid="{755321BC-C668-F042-8E31-CF64ED8C27AF}">
       <text>
         <r>
           <rPr>
@@ -2600,9 +2534,6 @@
     <t>vElevM</t>
   </si>
   <si>
-    <t>[archiveID]</t>
-  </si>
-  <si>
     <t>[pageNum]</t>
   </si>
   <si>
@@ -2700,6 +2631,9 @@
   </si>
   <si>
     <t>near Breezy Bay, Saturna  Island</t>
+  </si>
+  <si>
+    <t>idQualifier</t>
   </si>
 </sst>
 </file>
@@ -2776,7 +2710,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2803,6 +2737,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE2F0DB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2EFDA"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2835,7 +2775,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2852,6 +2792,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3169,26 +3110,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E2B542-A597-DF4D-A726-D9C00BB4087B}">
   <dimension ref="A1:AH64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="171" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="171" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="6.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="6.83203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="35.33203125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="24.83203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="7.5" style="3" customWidth="1"/>
-    <col min="7" max="7" width="24.6640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="11.83203125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="3"/>
-    <col min="10" max="10" width="14.33203125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="26" style="3" customWidth="1"/>
-    <col min="12" max="12" width="9" style="3" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="6.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="35.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="24.83203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="7.5" style="3" customWidth="1"/>
+    <col min="6" max="6" width="24.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="3"/>
+    <col min="9" max="9" width="14.33203125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="26" style="3" customWidth="1"/>
+    <col min="11" max="11" width="9" style="3" customWidth="1"/>
+    <col min="12" max="12" width="5.6640625" style="3" customWidth="1"/>
     <col min="13" max="13" width="16.83203125" style="3" customWidth="1"/>
     <col min="14" max="14" width="20.33203125" style="3" customWidth="1"/>
     <col min="15" max="15" width="21.5" style="3" customWidth="1"/>
@@ -3247,8 +3188,8 @@
       <c r="K1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="4" t="s">
-        <v>30</v>
+      <c r="L1" s="6" t="s">
+        <v>52</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>12</v>
@@ -3278,7 +3219,7 @@
         <v>10</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W1" s="2" t="s">
         <v>8</v>
@@ -3312,53 +3253,51 @@
       </c>
     </row>
     <row r="2" spans="1:34" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
-        <v>5</v>
-      </c>
-      <c r="B2">
+      <c r="A2">
         <v>10</v>
       </c>
-      <c r="C2"/>
+      <c r="B2"/>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
       <c r="D2" t="s">
         <v>36</v>
       </c>
       <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
         <v>37</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" s="3">
+        <v>1973039</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H2" s="3">
-        <v>1973039</v>
-      </c>
       <c r="I2" s="3" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="L2"/>
       <c r="W2"/>
       <c r="X2"/>
       <c r="AG2"/>
       <c r="AH2"/>
     </row>
     <row r="3" spans="1:34" ht="51" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
-        <v>5</v>
-      </c>
-      <c r="B3">
+      <c r="A3">
         <v>10</v>
       </c>
-      <c r="C3"/>
+      <c r="B3"/>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
       <c r="D3" t="s">
         <v>41</v>
       </c>
@@ -3366,213 +3305,215 @@
         <v>42</v>
       </c>
       <c r="F3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" t="s">
-        <v>42</v>
-      </c>
-      <c r="H3" s="3">
+        <v>41</v>
+      </c>
+      <c r="G3" s="3">
         <v>19730311</v>
       </c>
+      <c r="H3" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="I3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="K3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="L3"/>
       <c r="W3"/>
       <c r="X3"/>
       <c r="AH3"/>
     </row>
     <row r="4" spans="1:34" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
-        <v>5</v>
-      </c>
-      <c r="B4">
+      <c r="A4">
         <v>10</v>
       </c>
-      <c r="C4"/>
+      <c r="B4"/>
+      <c r="C4" t="s">
+        <v>43</v>
+      </c>
       <c r="D4" t="s">
         <v>44</v>
       </c>
       <c r="E4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="3">
+        <v>19730315</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L4"/>
+    </row>
+    <row r="5" spans="1:34" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>11</v>
+      </c>
+      <c r="B5"/>
+      <c r="C5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" t="s">
         <v>45</v>
       </c>
-      <c r="F4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="E5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" t="s">
         <v>45</v>
       </c>
-      <c r="H4" s="3">
-        <v>19730315</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J4" s="3" t="s">
+      <c r="G5" s="3">
+        <v>19730316</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:34" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
-        <v>5</v>
-      </c>
-      <c r="B5">
+      <c r="L5"/>
+      <c r="AH5"/>
+    </row>
+    <row r="6" spans="1:34" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>11</v>
       </c>
-      <c r="C5"/>
-      <c r="D5" t="s">
+      <c r="B6"/>
+      <c r="C6" t="s">
         <v>47</v>
       </c>
-      <c r="E5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" t="s">
-        <v>46</v>
-      </c>
-      <c r="H5" s="3">
-        <v>19730316</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH5"/>
-    </row>
-    <row r="6" spans="1:34" ht="51" x14ac:dyDescent="0.2">
-      <c r="B6">
-        <v>11</v>
-      </c>
-      <c r="C6"/>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E6" t="s">
         <v>48</v>
       </c>
       <c r="F6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="3">
+        <v>19730316</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6"/>
+      <c r="AF6" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H6" s="3">
-        <v>19730316</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AF6" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="AH6"/>
     </row>
     <row r="7" spans="1:34" ht="68" x14ac:dyDescent="0.2">
-      <c r="B7">
+      <c r="A7">
         <v>11</v>
       </c>
+      <c r="B7"/>
       <c r="C7"/>
       <c r="D7"/>
       <c r="E7"/>
       <c r="F7"/>
-      <c r="G7"/>
-      <c r="H7" s="3">
+      <c r="G7" s="3">
         <v>19730319</v>
       </c>
-      <c r="I7" s="3" t="s">
-        <v>52</v>
-      </c>
+      <c r="H7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="L7"/>
       <c r="O7" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A8"/>
       <c r="B8"/>
       <c r="C8"/>
       <c r="D8"/>
       <c r="E8"/>
       <c r="F8"/>
-      <c r="G8"/>
+      <c r="L8"/>
       <c r="AH8"/>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A9"/>
       <c r="B9"/>
       <c r="C9"/>
       <c r="D9"/>
       <c r="E9"/>
       <c r="F9"/>
-      <c r="G9"/>
+      <c r="L9"/>
       <c r="AH9"/>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A10"/>
       <c r="B10"/>
       <c r="C10"/>
       <c r="D10"/>
       <c r="E10"/>
       <c r="F10"/>
-      <c r="G10"/>
+      <c r="L10"/>
       <c r="AH10"/>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A11"/>
       <c r="B11"/>
       <c r="C11"/>
       <c r="D11"/>
       <c r="E11"/>
       <c r="F11"/>
-      <c r="G11"/>
+      <c r="L11"/>
       <c r="Q11"/>
       <c r="T11"/>
       <c r="AH11"/>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A12"/>
       <c r="B12"/>
       <c r="C12"/>
       <c r="D12"/>
       <c r="E12"/>
       <c r="F12"/>
-      <c r="G12"/>
+      <c r="L12"/>
       <c r="AH12"/>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A13"/>
       <c r="B13"/>
       <c r="C13"/>
       <c r="D13"/>
       <c r="E13"/>
       <c r="F13"/>
-      <c r="G13"/>
+      <c r="L13"/>
       <c r="Q13"/>
       <c r="T13"/>
       <c r="AB13"/>
@@ -3580,422 +3521,465 @@
       <c r="AH13"/>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A14"/>
       <c r="B14"/>
       <c r="C14"/>
       <c r="D14"/>
       <c r="E14"/>
       <c r="F14"/>
-      <c r="G14"/>
+      <c r="L14"/>
       <c r="Q14"/>
       <c r="T14"/>
       <c r="AH14"/>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A15"/>
       <c r="B15"/>
       <c r="C15"/>
       <c r="D15"/>
       <c r="E15"/>
       <c r="F15"/>
-      <c r="G15"/>
+      <c r="L15"/>
       <c r="Q15"/>
       <c r="T15"/>
       <c r="AH15"/>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A16"/>
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16"/>
       <c r="E16"/>
       <c r="F16"/>
-      <c r="G16"/>
+      <c r="L16"/>
       <c r="Q16"/>
       <c r="T16"/>
       <c r="AH16"/>
     </row>
-    <row r="17" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A17"/>
       <c r="B17"/>
       <c r="C17"/>
       <c r="D17"/>
       <c r="E17"/>
       <c r="F17"/>
-      <c r="G17"/>
+      <c r="L17"/>
       <c r="Q17"/>
       <c r="T17"/>
       <c r="AH17"/>
     </row>
-    <row r="18" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A18"/>
       <c r="B18"/>
       <c r="C18"/>
       <c r="D18"/>
       <c r="E18"/>
       <c r="F18"/>
-      <c r="G18"/>
+      <c r="L18"/>
       <c r="Q18"/>
       <c r="T18"/>
       <c r="AH18"/>
     </row>
-    <row r="19" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A19"/>
       <c r="B19"/>
       <c r="C19"/>
       <c r="D19"/>
       <c r="E19"/>
       <c r="F19"/>
-      <c r="G19"/>
+      <c r="L19"/>
       <c r="Q19"/>
       <c r="T19"/>
       <c r="AH19"/>
     </row>
-    <row r="20" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A20"/>
       <c r="B20"/>
       <c r="C20"/>
       <c r="D20"/>
       <c r="E20"/>
       <c r="F20"/>
-      <c r="G20"/>
+      <c r="L20"/>
       <c r="Q20"/>
       <c r="T20"/>
       <c r="AH20"/>
     </row>
-    <row r="21" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
       <c r="D21"/>
       <c r="E21"/>
       <c r="F21"/>
-      <c r="G21"/>
+      <c r="L21"/>
       <c r="Q21"/>
       <c r="T21"/>
       <c r="AH21"/>
     </row>
-    <row r="22" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
       <c r="D22"/>
       <c r="E22"/>
       <c r="F22"/>
-      <c r="G22"/>
+      <c r="L22"/>
       <c r="Q22"/>
       <c r="T22"/>
       <c r="AH22"/>
     </row>
-    <row r="23" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A23"/>
       <c r="B23"/>
       <c r="C23"/>
       <c r="D23"/>
       <c r="E23"/>
       <c r="F23"/>
-      <c r="G23"/>
+      <c r="L23"/>
       <c r="Q23"/>
       <c r="T23"/>
       <c r="AH23"/>
     </row>
-    <row r="24" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
       <c r="D24"/>
       <c r="E24"/>
       <c r="F24"/>
-      <c r="G24"/>
+      <c r="L24"/>
       <c r="Q24"/>
       <c r="T24"/>
       <c r="AH24"/>
     </row>
-    <row r="25" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
       <c r="D25"/>
       <c r="E25"/>
       <c r="F25"/>
-      <c r="G25"/>
+      <c r="L25"/>
       <c r="Q25"/>
       <c r="T25"/>
       <c r="AH25"/>
     </row>
-    <row r="26" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A26"/>
       <c r="B26"/>
       <c r="C26"/>
       <c r="D26"/>
       <c r="E26"/>
       <c r="F26"/>
-      <c r="G26"/>
+      <c r="L26"/>
       <c r="Q26"/>
       <c r="T26"/>
       <c r="AH26"/>
     </row>
-    <row r="27" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A27"/>
       <c r="B27"/>
       <c r="C27"/>
       <c r="D27"/>
       <c r="E27"/>
       <c r="F27"/>
-      <c r="G27"/>
+      <c r="L27"/>
       <c r="T27"/>
       <c r="AH27"/>
     </row>
-    <row r="28" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A28"/>
       <c r="B28"/>
       <c r="C28"/>
       <c r="D28"/>
       <c r="E28"/>
       <c r="F28"/>
-      <c r="G28"/>
+      <c r="L28"/>
       <c r="AH28"/>
     </row>
-    <row r="29" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A29"/>
       <c r="B29"/>
       <c r="C29"/>
       <c r="D29"/>
       <c r="E29"/>
       <c r="F29"/>
-      <c r="G29"/>
+      <c r="L29"/>
       <c r="AH29"/>
     </row>
-    <row r="30" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A30"/>
       <c r="B30"/>
       <c r="C30"/>
       <c r="D30"/>
       <c r="E30"/>
       <c r="F30"/>
-      <c r="G30"/>
+      <c r="L30"/>
       <c r="AH30"/>
     </row>
-    <row r="31" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A31"/>
       <c r="B31"/>
       <c r="C31"/>
       <c r="D31"/>
       <c r="E31"/>
       <c r="F31"/>
-      <c r="G31"/>
+      <c r="L31"/>
       <c r="AH31"/>
     </row>
-    <row r="32" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A32"/>
       <c r="B32"/>
-      <c r="C32"/>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A33"/>
       <c r="B33"/>
-      <c r="C33"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A34"/>
       <c r="B34"/>
-      <c r="C34"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A35"/>
       <c r="B35"/>
-      <c r="C35"/>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A36"/>
       <c r="B36"/>
-      <c r="C36"/>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A37"/>
       <c r="B37"/>
       <c r="C37"/>
       <c r="D37"/>
       <c r="E37"/>
       <c r="F37"/>
-      <c r="G37"/>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="L37"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A38"/>
       <c r="B38"/>
       <c r="C38"/>
       <c r="D38"/>
       <c r="E38"/>
       <c r="F38"/>
-      <c r="G38"/>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="L38"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A39"/>
       <c r="B39"/>
       <c r="C39"/>
       <c r="D39"/>
       <c r="E39"/>
       <c r="F39"/>
-      <c r="G39"/>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="L39"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A40"/>
       <c r="B40"/>
       <c r="C40"/>
       <c r="D40"/>
       <c r="E40"/>
       <c r="F40"/>
-      <c r="G40"/>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="L40"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A41"/>
       <c r="B41"/>
       <c r="C41"/>
       <c r="D41"/>
       <c r="E41"/>
       <c r="F41"/>
-      <c r="G41"/>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="L41"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A42"/>
       <c r="B42"/>
       <c r="C42"/>
       <c r="D42"/>
       <c r="E42"/>
       <c r="F42"/>
-      <c r="G42"/>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="L42"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A43"/>
       <c r="B43"/>
       <c r="C43"/>
       <c r="D43"/>
       <c r="E43"/>
       <c r="F43"/>
-      <c r="G43"/>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="L43"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A44"/>
       <c r="B44"/>
       <c r="C44"/>
       <c r="D44"/>
       <c r="E44"/>
       <c r="F44"/>
-      <c r="G44"/>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="L44"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A45"/>
       <c r="B45"/>
       <c r="C45"/>
       <c r="D45"/>
       <c r="E45"/>
       <c r="F45"/>
-      <c r="G45"/>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="L45"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A46"/>
       <c r="B46"/>
       <c r="C46"/>
       <c r="D46"/>
       <c r="E46"/>
       <c r="F46"/>
-      <c r="G46"/>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="L46"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A47"/>
       <c r="B47"/>
       <c r="C47"/>
       <c r="D47"/>
       <c r="E47"/>
       <c r="F47"/>
-      <c r="G47"/>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="L47"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A48"/>
       <c r="B48"/>
       <c r="C48"/>
       <c r="D48"/>
       <c r="E48"/>
       <c r="F48"/>
-      <c r="G48"/>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="L48"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A49"/>
       <c r="B49"/>
       <c r="C49"/>
       <c r="D49"/>
       <c r="E49"/>
       <c r="F49"/>
-      <c r="G49"/>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="L49"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A50"/>
       <c r="B50"/>
       <c r="C50"/>
       <c r="D50"/>
       <c r="E50"/>
       <c r="F50"/>
-      <c r="G50"/>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="L50"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A51"/>
       <c r="B51"/>
       <c r="C51"/>
       <c r="D51"/>
       <c r="E51"/>
       <c r="F51"/>
-      <c r="G51"/>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="L51"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A52"/>
       <c r="B52"/>
       <c r="C52"/>
       <c r="D52"/>
       <c r="E52"/>
       <c r="F52"/>
-      <c r="G52"/>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="L52"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A53"/>
       <c r="B53"/>
       <c r="C53"/>
       <c r="D53"/>
       <c r="E53"/>
       <c r="F53"/>
-      <c r="G53"/>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="L53"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A54"/>
       <c r="B54"/>
       <c r="C54"/>
       <c r="D54"/>
       <c r="E54"/>
       <c r="F54"/>
-      <c r="G54"/>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="L54"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A55"/>
       <c r="B55"/>
       <c r="C55"/>
       <c r="D55"/>
       <c r="E55"/>
       <c r="F55"/>
-      <c r="G55"/>
-    </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="L55"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A56"/>
       <c r="B56"/>
       <c r="C56"/>
       <c r="D56"/>
       <c r="E56"/>
       <c r="F56"/>
-      <c r="G56"/>
-    </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="L56"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A57"/>
       <c r="B57"/>
       <c r="C57"/>
       <c r="D57"/>
       <c r="E57"/>
       <c r="F57"/>
-      <c r="G57"/>
-    </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="L57"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A58"/>
       <c r="B58"/>
       <c r="C58"/>
       <c r="D58"/>
       <c r="E58"/>
       <c r="F58"/>
-      <c r="G58"/>
-    </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="L58"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A59"/>
       <c r="B59"/>
       <c r="C59"/>
       <c r="D59"/>
       <c r="E59"/>
       <c r="F59"/>
-      <c r="G59"/>
-    </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="L59"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A60"/>
       <c r="B60"/>
       <c r="C60"/>
       <c r="D60"/>
       <c r="E60"/>
       <c r="F60"/>
-      <c r="G60"/>
-    </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="L60"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A61"/>
       <c r="B61"/>
       <c r="C61"/>
       <c r="D61"/>
       <c r="E61"/>
       <c r="F61"/>
-      <c r="G61"/>
-    </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C62"/>
-    </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C63"/>
-    </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C64"/>
+      <c r="L61"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B62"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B63"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B64"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>

<commit_message>
completed dwc to RBCM format script
</commit_message>
<xml_diff>
--- a/data/digitized_data/occurrence_data/raw_data/HJ-5-occ-entry.xlsx
+++ b/data/digitized_data/occurrence_data/raw_data/HJ-5-occ-entry.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emma/Desktop/LDP Internship/Harvey_Janszen_Legacy_Project/data/digitized_data/occurrence_data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA84E9A-04A9-A743-8191-B2C6EE7DE6BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0275D6F7-6531-A741-8E24-B6BB5AA146DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15340" xr2:uid="{6CD260D0-3248-EC4C-A246-EE521030FA00}"/>
   </bookViews>
@@ -2630,7 +2630,7 @@
     <t>Saturna Island; Taylor Point</t>
   </si>
   <si>
-    <t>Saturna Island; near Breezy Bay</t>
+    <t>Saturna Island; Breezy Bay; near bay</t>
   </si>
 </sst>
 </file>
@@ -2809,7 +2809,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3097,7 +3097,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3107,10 +3107,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E2B542-A597-DF4D-A726-D9C00BB4087B}">
   <dimension ref="A1:AH64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="S3" sqref="S3"/>
+      <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="AH6"/>
     </row>
-    <row r="7" spans="1:34" ht="51" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:34" ht="68" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>11</v>
       </c>

</xml_diff>